<commit_message>
fix excel pull down error
</commit_message>
<xml_diff>
--- a/templates/community/MPIMP/MPIMP_Fernie_Mass_Spectrometry.xlsx
+++ b/templates/community/MPIMP/MPIMP_Fernie_Mass_Spectrometry.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbrilhaus/github/nfdi4plants/Swate-templates/templates/community/MPIMP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E422CAC4-C010-D344-AC0D-3BC348098774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0147868F-60CB-AC4D-A322-9235110CC461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23980" yWindow="-19840" windowWidth="27860" windowHeight="13520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23980" yWindow="-19840" windowWidth="27860" windowHeight="13520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mass spectrometry" sheetId="4" r:id="rId1"/>
@@ -199,7 +199,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="84">
   <si>
     <t>Source Name</t>
   </si>
@@ -298,9 +298,6 @@
   </si>
   <si>
     <t>1_neg.raw</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C17157</t>
   </si>
   <si>
     <t>Negative</t>
@@ -1086,31 +1083,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="40" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="33" customWidth="1"/>
+    <col min="4" max="4" width="40" customWidth="1"/>
     <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38.83203125" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="37.33203125" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="38.83203125" customWidth="1"/>
+    <col min="8" max="8" width="37.33203125" customWidth="1"/>
     <col min="9" max="9" width="38.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="40.33203125" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="35.33203125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="40.33203125" customWidth="1"/>
+    <col min="11" max="11" width="35.33203125" customWidth="1"/>
     <col min="12" max="12" width="35.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="31.1640625" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="38.33203125" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="31.1640625" customWidth="1"/>
+    <col min="14" max="14" width="38.33203125" customWidth="1"/>
     <col min="15" max="15" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="0" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="15.1640625" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="8.83203125" customWidth="1"/>
+    <col min="17" max="17" width="15.1640625" customWidth="1"/>
     <col min="18" max="18" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="0" hidden="1" customWidth="1"/>
+    <col min="19" max="20" width="8.83203125" customWidth="1"/>
     <col min="21" max="21" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1231,49 +1228,49 @@
         <v>19</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>19</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>19</v>
       </c>
       <c r="N3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1289,7 +1286,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -1302,107 +1299,107 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>49</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>51</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B7" s="8"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B9" s="7"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B10" s="7"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B11" s="8"/>
     </row>
     <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>18</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>20</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>19</v>
@@ -1413,91 +1410,91 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B15" s="8"/>
     </row>
     <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="9" t="s">
         <v>65</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>67</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B18" s="7"/>
     </row>
     <row r="19" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>70</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B20" s="7"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B21" s="7"/>
     </row>
     <row r="22" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>74</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>76</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>78</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B25" s="7"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B26" s="7"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B27" s="10"/>
     </row>

</xml_diff>